<commit_message>
Some fixes on the plotting functions for the paper
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
@@ -533,280 +533,96 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
-      <c r="A2">
-        <v>0.3300455909765285</v>
-      </c>
-      <c r="B2">
-        <v>0.3944846804539404</v>
-      </c>
-      <c r="C2">
-        <v>0.2826906343846102</v>
-      </c>
-      <c r="D2">
-        <v>0.3577864068138921</v>
-      </c>
-      <c r="E2">
-        <v>0.3011783511538316</v>
-      </c>
-      <c r="F2">
-        <v>7</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="K2">
-        <v>2.310319136835699</v>
-      </c>
-      <c r="L2">
-        <v>2.761392763177582</v>
-      </c>
-      <c r="M2">
-        <v>1.978834440692272</v>
-      </c>
-      <c r="N2">
-        <v>2.504504847697245</v>
-      </c>
-      <c r="O2">
-        <v>2.108248458076821</v>
-      </c>
-      <c r="P2">
-        <v>63.915</v>
-      </c>
-      <c r="Q2">
-        <v>80.85574894288354</v>
-      </c>
-      <c r="R2">
-        <v>48.11247350763706</v>
-      </c>
-      <c r="S2">
-        <v>72.67917486573398</v>
-      </c>
-      <c r="T2">
-        <v>54.97238490226889</v>
-      </c>
-      <c r="U2">
-        <v>0.203534735826472</v>
-      </c>
-      <c r="V2">
-        <v>0.2686067778606374</v>
-      </c>
-      <c r="W2">
-        <v>0.1490367641532766</v>
-      </c>
-      <c r="X2">
-        <v>0.2359845531166401</v>
-      </c>
-      <c r="Y2">
-        <v>0.1718837203704537</v>
-      </c>
-      <c r="Z2">
-        <v>0.8593985364230792</v>
-      </c>
-      <c r="AA2">
-        <v>0.9217917025025576</v>
-      </c>
-      <c r="AB2">
-        <v>0.7920693401785304</v>
-      </c>
-      <c r="AC2">
-        <v>0.8935779657913432</v>
-      </c>
-      <c r="AD2">
-        <v>0.8223789133325942</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30">
-      <c r="A3">
-        <v>0.33</v>
-      </c>
-      <c r="B3">
-        <v>0.33</v>
-      </c>
-      <c r="C3">
-        <v>0.33</v>
-      </c>
-      <c r="D3">
-        <v>0.33</v>
-      </c>
-      <c r="E3">
-        <v>0.33</v>
-      </c>
-      <c r="F3">
-        <v>7.009742652918423</v>
-      </c>
-      <c r="G3">
-        <v>9.136180526005635</v>
-      </c>
-      <c r="H3">
-        <v>5.449700167756184</v>
-      </c>
-      <c r="I3">
-        <v>7.899019129571238</v>
-      </c>
-      <c r="J3">
-        <v>6.062769355814714</v>
-      </c>
-      <c r="K3">
-        <v>2.31321507546308</v>
-      </c>
-      <c r="L3">
-        <v>3.014939573581859</v>
-      </c>
-      <c r="M3">
-        <v>1.798401055359541</v>
-      </c>
-      <c r="N3">
-        <v>2.606676312758509</v>
-      </c>
-      <c r="O3">
-        <v>2.000713887418856</v>
-      </c>
-      <c r="P3">
-        <v>63.8196</v>
-      </c>
-      <c r="Q3">
-        <v>75.10459226751333</v>
-      </c>
-      <c r="R3">
-        <v>55.46934830353591</v>
-      </c>
-      <c r="S3">
-        <v>69.0990389572992</v>
-      </c>
-      <c r="T3">
-        <v>58.93864725208331</v>
-      </c>
-      <c r="U3">
-        <v>0.2025441208058643</v>
-      </c>
-      <c r="V3">
-        <v>0.2997073702641776</v>
-      </c>
-      <c r="W3">
-        <v>0.1165867951390386</v>
-      </c>
-      <c r="X3">
-        <v>0.2519455428458237</v>
-      </c>
-      <c r="Y3">
-        <v>0.1532404587508523</v>
-      </c>
-      <c r="Z3">
-        <v>0.8531899322856674</v>
-      </c>
-      <c r="AA3">
-        <v>0.9434745729198976</v>
-      </c>
-      <c r="AB3">
-        <v>0.735104523875359</v>
-      </c>
-      <c r="AC3">
-        <v>0.9049573714047749</v>
-      </c>
-      <c r="AD3">
-        <v>0.7923088059672058</v>
-      </c>
-    </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>0.3301962166185204</v>
+        <v>0.3300896489316999</v>
       </c>
       <c r="B4">
-        <v>0.3934807693118949</v>
+        <v>0.3937716913375339</v>
       </c>
       <c r="C4">
-        <v>0.2819766121176503</v>
+        <v>0.2831114229638663</v>
       </c>
       <c r="D4">
-        <v>0.3573965907731411</v>
+        <v>0.3572739247688735</v>
       </c>
       <c r="E4">
-        <v>0.3018455481879944</v>
+        <v>0.3016866985809186</v>
       </c>
       <c r="F4">
-        <v>7.011243773908282</v>
+        <v>7.005345674098685</v>
       </c>
       <c r="G4">
-        <v>9.132221970617771</v>
+        <v>9.155225268991765</v>
       </c>
       <c r="H4">
-        <v>5.46068751056686</v>
+        <v>5.443870653969218</v>
       </c>
       <c r="I4">
-        <v>7.901779989725624</v>
+        <v>7.911868107462011</v>
       </c>
       <c r="J4">
-        <v>6.058375804924896</v>
+        <v>6.057471535817356</v>
       </c>
       <c r="K4">
-        <v>2.314506829182654</v>
+        <v>2.312451696222781</v>
       </c>
       <c r="L4">
-        <v>3.149350034713079</v>
+        <v>3.165432737870411</v>
       </c>
       <c r="M4">
-        <v>1.713246406141923</v>
+        <v>1.704226334517611</v>
       </c>
       <c r="N4">
-        <v>2.665607159684349</v>
+        <v>2.663326251156235</v>
       </c>
       <c r="O4">
-        <v>1.942507817848142</v>
+        <v>1.942531147614155</v>
       </c>
       <c r="P4">
-        <v>65.02589999999999</v>
+        <v>65.10586000000001</v>
       </c>
       <c r="Q4">
-        <v>90.88740254183415</v>
+        <v>90.81940183026543</v>
       </c>
       <c r="R4">
-        <v>47.44888235059661</v>
+        <v>47.44349024310426</v>
       </c>
       <c r="S4">
-        <v>74.33499904736274</v>
+        <v>74.42357440141171</v>
       </c>
       <c r="T4">
-        <v>54.81768155198472</v>
+        <v>54.8440184763783</v>
       </c>
       <c r="U4">
-        <v>0.2017260414117216</v>
+        <v>0.2013384968688031</v>
       </c>
       <c r="V4">
-        <v>0.316466822635505</v>
+        <v>0.317510705356708</v>
       </c>
       <c r="W4">
-        <v>0.1004689967042615</v>
+        <v>0.09932328267674136</v>
       </c>
       <c r="X4">
-        <v>0.2602173189274399</v>
+        <v>0.2602566524088788</v>
       </c>
       <c r="Y4">
-        <v>0.1434159974825161</v>
+        <v>0.1427160606128784</v>
       </c>
       <c r="Z4">
-        <v>0.8485328141951699</v>
+        <v>0.8478579537441078</v>
       </c>
       <c r="AA4">
-        <v>0.9540544445646497</v>
+        <v>0.9546501438494737</v>
       </c>
       <c r="AB4">
-        <v>0.7002954964736789</v>
+        <v>0.697919396871762</v>
       </c>
       <c r="AC4">
-        <v>0.9098458983380742</v>
+        <v>0.9097483621377701</v>
       </c>
       <c r="AD4">
-        <v>0.7740832814256954</v>
+        <v>0.7726976537329295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more fixes for paper
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
@@ -533,96 +533,280 @@
         <v>29</v>
       </c>
     </row>
+    <row r="2" spans="1:30">
+      <c r="A2">
+        <v>0.3301136626125567</v>
+      </c>
+      <c r="B2">
+        <v>0.3949069889952284</v>
+      </c>
+      <c r="C2">
+        <v>0.2832973020472173</v>
+      </c>
+      <c r="D2">
+        <v>0.3571804451842914</v>
+      </c>
+      <c r="E2">
+        <v>0.3017493060930475</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <v>2.310795638287897</v>
+      </c>
+      <c r="L2">
+        <v>2.764348922966599</v>
+      </c>
+      <c r="M2">
+        <v>1.983081114330521</v>
+      </c>
+      <c r="N2">
+        <v>2.50026311629004</v>
+      </c>
+      <c r="O2">
+        <v>2.112245142651332</v>
+      </c>
+      <c r="P2">
+        <v>63.88048</v>
+      </c>
+      <c r="Q2">
+        <v>80.64758792200021</v>
+      </c>
+      <c r="R2">
+        <v>48.10386154325745</v>
+      </c>
+      <c r="S2">
+        <v>72.54372444754591</v>
+      </c>
+      <c r="T2">
+        <v>55.00654197501315</v>
+      </c>
+      <c r="U2">
+        <v>0.203616653773568</v>
+      </c>
+      <c r="V2">
+        <v>0.2687802782889044</v>
+      </c>
+      <c r="W2">
+        <v>0.1494746064757829</v>
+      </c>
+      <c r="X2">
+        <v>0.2357895216797287</v>
+      </c>
+      <c r="Y2">
+        <v>0.1723380961865035</v>
+      </c>
+      <c r="Z2">
+        <v>0.8595319604176113</v>
+      </c>
+      <c r="AA2">
+        <v>0.9218073099881111</v>
+      </c>
+      <c r="AB2">
+        <v>0.7929035260783918</v>
+      </c>
+      <c r="AC2">
+        <v>0.8933913491789289</v>
+      </c>
+      <c r="AD2">
+        <v>0.822971758626735</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3">
+        <v>0.33</v>
+      </c>
+      <c r="B3">
+        <v>0.33</v>
+      </c>
+      <c r="C3">
+        <v>0.33</v>
+      </c>
+      <c r="D3">
+        <v>0.33</v>
+      </c>
+      <c r="E3">
+        <v>0.33</v>
+      </c>
+      <c r="F3">
+        <v>7.008650454676773</v>
+      </c>
+      <c r="G3">
+        <v>9.137338641110436</v>
+      </c>
+      <c r="H3">
+        <v>5.443269109730695</v>
+      </c>
+      <c r="I3">
+        <v>7.917152192314232</v>
+      </c>
+      <c r="J3">
+        <v>6.061317022253602</v>
+      </c>
+      <c r="K3">
+        <v>2.312854650043335</v>
+      </c>
+      <c r="L3">
+        <v>3.015321751566444</v>
+      </c>
+      <c r="M3">
+        <v>1.796278806211129</v>
+      </c>
+      <c r="N3">
+        <v>2.612660223463696</v>
+      </c>
+      <c r="O3">
+        <v>2.000234617343688</v>
+      </c>
+      <c r="P3">
+        <v>63.8488</v>
+      </c>
+      <c r="Q3">
+        <v>75.21552451439547</v>
+      </c>
+      <c r="R3">
+        <v>55.42784932428966</v>
+      </c>
+      <c r="S3">
+        <v>69.18625840385873</v>
+      </c>
+      <c r="T3">
+        <v>58.90981425312337</v>
+      </c>
+      <c r="U3">
+        <v>0.202436494678118</v>
+      </c>
+      <c r="V3">
+        <v>0.300552560485084</v>
+      </c>
+      <c r="W3">
+        <v>0.116192452246413</v>
+      </c>
+      <c r="X3">
+        <v>0.2524199123774446</v>
+      </c>
+      <c r="Y3">
+        <v>0.1526893179694813</v>
+      </c>
+      <c r="Z3">
+        <v>0.8528999012808594</v>
+      </c>
+      <c r="AA3">
+        <v>0.9440024691536069</v>
+      </c>
+      <c r="AB3">
+        <v>0.7341154569326024</v>
+      </c>
+      <c r="AC3">
+        <v>0.9052864392390564</v>
+      </c>
+      <c r="AD3">
+        <v>0.7914206999631612</v>
+      </c>
+    </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>0.3300896489316999</v>
+        <v>0.3300789700090945</v>
       </c>
       <c r="B4">
-        <v>0.3937716913375339</v>
+        <v>0.3943883010179898</v>
       </c>
       <c r="C4">
-        <v>0.2831114229638663</v>
+        <v>0.2833683820696578</v>
       </c>
       <c r="D4">
-        <v>0.3572739247688735</v>
+        <v>0.3570496897887267</v>
       </c>
       <c r="E4">
-        <v>0.3016866985809186</v>
+        <v>0.3017349428211397</v>
       </c>
       <c r="F4">
-        <v>7.005345674098685</v>
+        <v>7.006449683098982</v>
       </c>
       <c r="G4">
-        <v>9.155225268991765</v>
+        <v>9.127987050857911</v>
       </c>
       <c r="H4">
-        <v>5.443870653969218</v>
+        <v>5.431402308235739</v>
       </c>
       <c r="I4">
-        <v>7.911868107462011</v>
+        <v>7.911817098952892</v>
       </c>
       <c r="J4">
-        <v>6.057471535817356</v>
+        <v>6.059075348741236</v>
       </c>
       <c r="K4">
-        <v>2.312451696222781</v>
+        <v>2.312727900809143</v>
       </c>
       <c r="L4">
-        <v>3.165432737870411</v>
+        <v>3.155615094726688</v>
       </c>
       <c r="M4">
-        <v>1.704226334517611</v>
+        <v>1.703826992705189</v>
       </c>
       <c r="N4">
-        <v>2.663326251156235</v>
+        <v>2.666498669303904</v>
       </c>
       <c r="O4">
-        <v>1.942531147614155</v>
+        <v>1.943636146755307</v>
       </c>
       <c r="P4">
-        <v>65.10586000000001</v>
+        <v>65.10521</v>
       </c>
       <c r="Q4">
-        <v>90.81940183026543</v>
+        <v>90.68672292392961</v>
       </c>
       <c r="R4">
-        <v>47.44349024310426</v>
+        <v>47.36474784479361</v>
       </c>
       <c r="S4">
-        <v>74.42357440141171</v>
+        <v>75.00734373692225</v>
       </c>
       <c r="T4">
-        <v>54.8440184763783</v>
+        <v>54.9017405427993</v>
       </c>
       <c r="U4">
-        <v>0.2013384968688031</v>
+        <v>0.2013971555282028</v>
       </c>
       <c r="V4">
-        <v>0.317510705356708</v>
+        <v>0.3169361038270316</v>
       </c>
       <c r="W4">
-        <v>0.09932328267674136</v>
+        <v>0.09917400691363822</v>
       </c>
       <c r="X4">
-        <v>0.2602566524088788</v>
+        <v>0.2602388622497128</v>
       </c>
       <c r="Y4">
-        <v>0.1427160606128784</v>
+        <v>0.142669912107736</v>
       </c>
       <c r="Z4">
-        <v>0.8478579537441078</v>
+        <v>0.8479147069084788</v>
       </c>
       <c r="AA4">
-        <v>0.9546501438494737</v>
+        <v>0.9544819082535033</v>
       </c>
       <c r="AB4">
-        <v>0.697919396871762</v>
+        <v>0.6971593999335332</v>
       </c>
       <c r="AC4">
-        <v>0.9097483621377701</v>
+        <v>0.9097051757792216</v>
       </c>
       <c r="AD4">
-        <v>0.7726976537329295</v>
+        <v>0.7726048598037696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating plotting functions and simulation parameters to match paper
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
@@ -533,280 +533,96 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
-      <c r="A2">
-        <v>0.3301136626125567</v>
-      </c>
-      <c r="B2">
-        <v>0.3949069889952284</v>
-      </c>
-      <c r="C2">
-        <v>0.2832973020472173</v>
-      </c>
-      <c r="D2">
-        <v>0.3571804451842914</v>
-      </c>
-      <c r="E2">
-        <v>0.3017493060930475</v>
-      </c>
-      <c r="F2">
-        <v>7</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="K2">
-        <v>2.310795638287897</v>
-      </c>
-      <c r="L2">
-        <v>2.764348922966599</v>
-      </c>
-      <c r="M2">
-        <v>1.983081114330521</v>
-      </c>
-      <c r="N2">
-        <v>2.50026311629004</v>
-      </c>
-      <c r="O2">
-        <v>2.112245142651332</v>
-      </c>
-      <c r="P2">
-        <v>63.88048</v>
-      </c>
-      <c r="Q2">
-        <v>80.64758792200021</v>
-      </c>
-      <c r="R2">
-        <v>48.10386154325745</v>
-      </c>
-      <c r="S2">
-        <v>72.54372444754591</v>
-      </c>
-      <c r="T2">
-        <v>55.00654197501315</v>
-      </c>
-      <c r="U2">
-        <v>0.203616653773568</v>
-      </c>
-      <c r="V2">
-        <v>0.2687802782889044</v>
-      </c>
-      <c r="W2">
-        <v>0.1494746064757829</v>
-      </c>
-      <c r="X2">
-        <v>0.2357895216797287</v>
-      </c>
-      <c r="Y2">
-        <v>0.1723380961865035</v>
-      </c>
-      <c r="Z2">
-        <v>0.8595319604176113</v>
-      </c>
-      <c r="AA2">
-        <v>0.9218073099881111</v>
-      </c>
-      <c r="AB2">
-        <v>0.7929035260783918</v>
-      </c>
-      <c r="AC2">
-        <v>0.8933913491789289</v>
-      </c>
-      <c r="AD2">
-        <v>0.822971758626735</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30">
-      <c r="A3">
-        <v>0.33</v>
-      </c>
-      <c r="B3">
-        <v>0.33</v>
-      </c>
-      <c r="C3">
-        <v>0.33</v>
-      </c>
-      <c r="D3">
-        <v>0.33</v>
-      </c>
-      <c r="E3">
-        <v>0.33</v>
-      </c>
-      <c r="F3">
-        <v>7.008650454676773</v>
-      </c>
-      <c r="G3">
-        <v>9.137338641110436</v>
-      </c>
-      <c r="H3">
-        <v>5.443269109730695</v>
-      </c>
-      <c r="I3">
-        <v>7.917152192314232</v>
-      </c>
-      <c r="J3">
-        <v>6.061317022253602</v>
-      </c>
-      <c r="K3">
-        <v>2.312854650043335</v>
-      </c>
-      <c r="L3">
-        <v>3.015321751566444</v>
-      </c>
-      <c r="M3">
-        <v>1.796278806211129</v>
-      </c>
-      <c r="N3">
-        <v>2.612660223463696</v>
-      </c>
-      <c r="O3">
-        <v>2.000234617343688</v>
-      </c>
-      <c r="P3">
-        <v>63.8488</v>
-      </c>
-      <c r="Q3">
-        <v>75.21552451439547</v>
-      </c>
-      <c r="R3">
-        <v>55.42784932428966</v>
-      </c>
-      <c r="S3">
-        <v>69.18625840385873</v>
-      </c>
-      <c r="T3">
-        <v>58.90981425312337</v>
-      </c>
-      <c r="U3">
-        <v>0.202436494678118</v>
-      </c>
-      <c r="V3">
-        <v>0.300552560485084</v>
-      </c>
-      <c r="W3">
-        <v>0.116192452246413</v>
-      </c>
-      <c r="X3">
-        <v>0.2524199123774446</v>
-      </c>
-      <c r="Y3">
-        <v>0.1526893179694813</v>
-      </c>
-      <c r="Z3">
-        <v>0.8528999012808594</v>
-      </c>
-      <c r="AA3">
-        <v>0.9440024691536069</v>
-      </c>
-      <c r="AB3">
-        <v>0.7341154569326024</v>
-      </c>
-      <c r="AC3">
-        <v>0.9052864392390564</v>
-      </c>
-      <c r="AD3">
-        <v>0.7914206999631612</v>
-      </c>
-    </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>0.3300789700090945</v>
+        <v>0.3299583781535884</v>
       </c>
       <c r="B4">
-        <v>0.3943883010179898</v>
+        <v>0.3934589318997483</v>
       </c>
       <c r="C4">
-        <v>0.2833683820696578</v>
+        <v>0.2830644034726374</v>
       </c>
       <c r="D4">
-        <v>0.3570496897887267</v>
+        <v>0.3572424448617109</v>
       </c>
       <c r="E4">
-        <v>0.3017349428211397</v>
+        <v>0.3017340007039827</v>
       </c>
       <c r="F4">
-        <v>7.006449683098982</v>
+        <v>7.009341074576589</v>
       </c>
       <c r="G4">
-        <v>9.127987050857911</v>
+        <v>9.144184282807482</v>
       </c>
       <c r="H4">
-        <v>5.431402308235739</v>
+        <v>5.437165512591095</v>
       </c>
       <c r="I4">
-        <v>7.911817098952892</v>
+        <v>7.920617889073113</v>
       </c>
       <c r="J4">
-        <v>6.059075348741236</v>
+        <v>6.060652977894222</v>
       </c>
       <c r="K4">
-        <v>2.312727900809143</v>
+        <v>2.312775817796077</v>
       </c>
       <c r="L4">
-        <v>3.155615094726688</v>
+        <v>3.160239842787972</v>
       </c>
       <c r="M4">
-        <v>1.703826992705189</v>
+        <v>1.702839254565729</v>
       </c>
       <c r="N4">
-        <v>2.666498669303904</v>
+        <v>2.665294820428289</v>
       </c>
       <c r="O4">
-        <v>1.943636146755307</v>
+        <v>1.944296884611536</v>
       </c>
       <c r="P4">
-        <v>65.10521</v>
+        <v>65.12430999999999</v>
       </c>
       <c r="Q4">
-        <v>90.68672292392961</v>
+        <v>90.9821292620059</v>
       </c>
       <c r="R4">
-        <v>47.36474784479361</v>
+        <v>47.49237712278485</v>
       </c>
       <c r="S4">
-        <v>75.00734373692225</v>
+        <v>74.48617558543192</v>
       </c>
       <c r="T4">
-        <v>54.9017405427993</v>
+        <v>54.84334922681201</v>
       </c>
       <c r="U4">
-        <v>0.2013971555282028</v>
+        <v>0.2013988016168057</v>
       </c>
       <c r="V4">
-        <v>0.3169361038270316</v>
+        <v>0.3171759848229364</v>
       </c>
       <c r="W4">
-        <v>0.09917400691363822</v>
+        <v>0.09930305172662894</v>
       </c>
       <c r="X4">
-        <v>0.2602388622497128</v>
+        <v>0.2602628764248707</v>
       </c>
       <c r="Y4">
-        <v>0.142669912107736</v>
+        <v>0.1427292029185049</v>
       </c>
       <c r="Z4">
-        <v>0.8479147069084788</v>
+        <v>0.8479314086336348</v>
       </c>
       <c r="AA4">
-        <v>0.9544819082535033</v>
+        <v>0.9545603526709378</v>
       </c>
       <c r="AB4">
-        <v>0.6971593999335332</v>
+        <v>0.6976235327873144</v>
       </c>
       <c r="AC4">
-        <v>0.9097051757792216</v>
+        <v>0.9097342760093722</v>
       </c>
       <c r="AD4">
-        <v>0.7726048598037696</v>
+        <v>0.7727318940014264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest updates and plots for paper
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
@@ -535,94 +535,94 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>0.3299583781535884</v>
+        <v>0.3300724615171935</v>
       </c>
       <c r="B4">
-        <v>0.3934589318997483</v>
+        <v>0.3939180674855193</v>
       </c>
       <c r="C4">
-        <v>0.2830644034726374</v>
+        <v>0.28315744431636</v>
       </c>
       <c r="D4">
-        <v>0.3572424448617109</v>
+        <v>0.3572073749129407</v>
       </c>
       <c r="E4">
-        <v>0.3017340007039827</v>
+        <v>0.3017672444927606</v>
       </c>
       <c r="F4">
-        <v>7.009341074576589</v>
+        <v>7.009940117459498</v>
       </c>
       <c r="G4">
-        <v>9.144184282807482</v>
+        <v>9.14049226783138</v>
       </c>
       <c r="H4">
-        <v>5.437165512591095</v>
+        <v>5.44428906282274</v>
       </c>
       <c r="I4">
-        <v>7.920617889073113</v>
+        <v>7.916869781435245</v>
       </c>
       <c r="J4">
-        <v>6.060652977894222</v>
+        <v>6.061858984930184</v>
       </c>
       <c r="K4">
-        <v>2.312775817796077</v>
+        <v>2.313796406217068</v>
       </c>
       <c r="L4">
-        <v>3.160239842787972</v>
+        <v>3.157439112056929</v>
       </c>
       <c r="M4">
-        <v>1.702839254565729</v>
+        <v>1.704766793562185</v>
       </c>
       <c r="N4">
-        <v>2.665294820428289</v>
+        <v>2.666677956112652</v>
       </c>
       <c r="O4">
-        <v>1.944296884611536</v>
+        <v>1.945404950478435</v>
       </c>
       <c r="P4">
-        <v>65.12430999999999</v>
+        <v>65.082931</v>
       </c>
       <c r="Q4">
-        <v>90.9821292620059</v>
+        <v>90.80950833653185</v>
       </c>
       <c r="R4">
-        <v>47.49237712278485</v>
+        <v>47.4482028160903</v>
       </c>
       <c r="S4">
-        <v>74.48617558543192</v>
+        <v>74.37772062264614</v>
       </c>
       <c r="T4">
-        <v>54.84334922681201</v>
+        <v>54.8171366293158</v>
       </c>
       <c r="U4">
-        <v>0.2013988016168057</v>
+        <v>0.2015597452512233</v>
       </c>
       <c r="V4">
-        <v>0.3171759848229364</v>
+        <v>0.3171580079148343</v>
       </c>
       <c r="W4">
-        <v>0.09930305172662894</v>
+        <v>0.09954007807863229</v>
       </c>
       <c r="X4">
-        <v>0.2602628764248707</v>
+        <v>0.2604303568272447</v>
       </c>
       <c r="Y4">
-        <v>0.1427292029185049</v>
+        <v>0.1428659843637737</v>
       </c>
       <c r="Z4">
-        <v>0.8479314086336348</v>
+        <v>0.8481391630065199</v>
       </c>
       <c r="AA4">
-        <v>0.9545603526709378</v>
+        <v>0.9544990526690307</v>
       </c>
       <c r="AB4">
-        <v>0.6976235327873144</v>
+        <v>0.6981896653970183</v>
       </c>
       <c r="AC4">
-        <v>0.9097342760093722</v>
+        <v>0.9099013217487522</v>
       </c>
       <c r="AD4">
-        <v>0.7727318940014264</v>
+        <v>0.7730145981012134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some changes and updated notes for distributions
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
@@ -533,280 +533,96 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
-      <c r="A2">
-        <v>0.3299830562023636</v>
-      </c>
-      <c r="B2">
-        <v>0.4386365809456049</v>
-      </c>
-      <c r="C2">
-        <v>0.2684138756856539</v>
-      </c>
-      <c r="D2">
-        <v>0.393336293331695</v>
-      </c>
-      <c r="E2">
-        <v>0.283151041482563</v>
-      </c>
-      <c r="F2">
-        <v>7</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="K2">
-        <v>2.309881393416545</v>
-      </c>
-      <c r="L2">
-        <v>3.070456066619235</v>
-      </c>
-      <c r="M2">
-        <v>1.878897129799577</v>
-      </c>
-      <c r="N2">
-        <v>2.753354053321865</v>
-      </c>
-      <c r="O2">
-        <v>1.982057290377941</v>
-      </c>
-      <c r="P2">
-        <v>63.90929</v>
-      </c>
-      <c r="Q2">
-        <v>80.75389814919497</v>
-      </c>
-      <c r="R2">
-        <v>48.29881550823153</v>
-      </c>
-      <c r="S2">
-        <v>72.57904959339953</v>
-      </c>
-      <c r="T2">
-        <v>55.08549281762739</v>
-      </c>
-      <c r="U2">
-        <v>0.2034905141335044</v>
-      </c>
-      <c r="V2">
-        <v>0.2677275618652732</v>
-      </c>
-      <c r="W2">
-        <v>0.1492419017758285</v>
-      </c>
-      <c r="X2">
-        <v>0.2354454045211803</v>
-      </c>
-      <c r="Y2">
-        <v>0.1722097052987395</v>
-      </c>
-      <c r="Z2">
-        <v>0.8594247681719996</v>
-      </c>
-      <c r="AA2">
-        <v>0.921078679322038</v>
-      </c>
-      <c r="AB2">
-        <v>0.7924626821473525</v>
-      </c>
-      <c r="AC2">
-        <v>0.8931149449609513</v>
-      </c>
-      <c r="AD2">
-        <v>0.8228209416250843</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30">
-      <c r="A3">
-        <v>0.33</v>
-      </c>
-      <c r="B3">
-        <v>0.33</v>
-      </c>
-      <c r="C3">
-        <v>0.33</v>
-      </c>
-      <c r="D3">
-        <v>0.33</v>
-      </c>
-      <c r="E3">
-        <v>0.33</v>
-      </c>
-      <c r="F3">
-        <v>7.006584745387602</v>
-      </c>
-      <c r="G3">
-        <v>10.60790787652156</v>
-      </c>
-      <c r="H3">
-        <v>4.925882002000065</v>
-      </c>
-      <c r="I3">
-        <v>9.142436822103727</v>
-      </c>
-      <c r="J3">
-        <v>5.438013145935202</v>
-      </c>
-      <c r="K3">
-        <v>2.312172965977909</v>
-      </c>
-      <c r="L3">
-        <v>3.500609599252114</v>
-      </c>
-      <c r="M3">
-        <v>1.625541060660021</v>
-      </c>
-      <c r="N3">
-        <v>3.01700415129423</v>
-      </c>
-      <c r="O3">
-        <v>1.794544338158617</v>
-      </c>
-      <c r="P3">
-        <v>63.87335</v>
-      </c>
-      <c r="Q3">
-        <v>75.28546872997143</v>
-      </c>
-      <c r="R3">
-        <v>55.40921738845646</v>
-      </c>
-      <c r="S3">
-        <v>69.2493885609226</v>
-      </c>
-      <c r="T3">
-        <v>58.89556948997839</v>
-      </c>
-      <c r="U3">
-        <v>0.2023037194233211</v>
-      </c>
-      <c r="V3">
-        <v>0.3008321349293454</v>
-      </c>
-      <c r="W3">
-        <v>0.1160078745524592</v>
-      </c>
-      <c r="X3">
-        <v>0.2526450656762114</v>
-      </c>
-      <c r="Y3">
-        <v>0.1522806950574559</v>
-      </c>
-      <c r="Z3">
-        <v>0.8526586651159245</v>
-      </c>
-      <c r="AA3">
-        <v>0.9441666153693865</v>
-      </c>
-      <c r="AB3">
-        <v>0.7335630090920561</v>
-      </c>
-      <c r="AC3">
-        <v>0.9054559761623971</v>
-      </c>
-      <c r="AD3">
-        <v>0.7907872241351499</v>
-      </c>
-    </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>0.330020523265408</v>
+        <v>0.3300548414179534</v>
       </c>
       <c r="B4">
-        <v>0.4404016719778163</v>
+        <v>0.438391105008159</v>
       </c>
       <c r="C4">
-        <v>0.2679345486534457</v>
+        <v>0.2679979988735469</v>
       </c>
       <c r="D4">
-        <v>0.3941200762398092</v>
+        <v>0.3937391041631541</v>
       </c>
       <c r="E4">
-        <v>0.2830483831412635</v>
+        <v>0.2828853923370157</v>
       </c>
       <c r="F4">
-        <v>7.011955677356151</v>
+        <v>7.007322609896816</v>
       </c>
       <c r="G4">
-        <v>10.60362528640664</v>
+        <v>10.59244524579269</v>
       </c>
       <c r="H4">
-        <v>4.94778129737217</v>
+        <v>4.943887736082482</v>
       </c>
       <c r="I4">
-        <v>9.134376319648373</v>
+        <v>9.156663608614821</v>
       </c>
       <c r="J4">
-        <v>5.448272680657131</v>
+        <v>5.454697200150446</v>
       </c>
       <c r="K4">
-        <v>2.313934175696478</v>
+        <v>2.312828591780329</v>
       </c>
       <c r="L4">
-        <v>3.783168462490773</v>
+        <v>3.776206511706212</v>
       </c>
       <c r="M4">
-        <v>1.510440821957939</v>
+        <v>1.504166808897832</v>
       </c>
       <c r="N4">
-        <v>3.158395569536554</v>
+        <v>3.157386487208637</v>
       </c>
       <c r="O4">
-        <v>1.706225323334587</v>
+        <v>1.705213153564048</v>
       </c>
       <c r="P4">
-        <v>65.08046</v>
+        <v>65.09828</v>
       </c>
       <c r="Q4">
-        <v>90.71235680793677</v>
+        <v>90.86152396822476</v>
       </c>
       <c r="R4">
-        <v>47.44549773314107</v>
+        <v>47.47755553305626</v>
       </c>
       <c r="S4">
-        <v>74.46911618481222</v>
+        <v>74.3787818779372</v>
       </c>
       <c r="T4">
-        <v>54.8428957785704</v>
+        <v>54.8664087005132</v>
       </c>
       <c r="U4">
-        <v>0.2016027257065575</v>
+        <v>0.2014188176078627</v>
       </c>
       <c r="V4">
-        <v>0.3168441712345526</v>
+        <v>0.3170577056105753</v>
       </c>
       <c r="W4">
-        <v>0.09975734422794665</v>
+        <v>0.09951348041250996</v>
       </c>
       <c r="X4">
-        <v>0.2602906484495348</v>
+        <v>0.2601819905801135</v>
       </c>
       <c r="Y4">
-        <v>0.1430569980547441</v>
+        <v>0.1428659134014484</v>
       </c>
       <c r="Z4">
-        <v>0.8482607044897501</v>
+        <v>0.8480062911440618</v>
       </c>
       <c r="AA4">
-        <v>0.9543292277604642</v>
+        <v>0.9544705393367487</v>
       </c>
       <c r="AB4">
-        <v>0.6987064122251661</v>
+        <v>0.6981762718042079</v>
       </c>
       <c r="AC4">
-        <v>0.9098170295651775</v>
+        <v>0.9096999253447704</v>
       </c>
       <c r="AD4">
-        <v>0.773372062971861</v>
+        <v>0.7729972162013145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes for paper plots
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
@@ -533,96 +533,280 @@
         <v>29</v>
       </c>
     </row>
+    <row r="2" spans="1:30">
+      <c r="A2">
+        <v>0.330119001686855</v>
+      </c>
+      <c r="B2">
+        <v>0.4392605252959991</v>
+      </c>
+      <c r="C2">
+        <v>0.2681703911211314</v>
+      </c>
+      <c r="D2">
+        <v>0.3937878288901468</v>
+      </c>
+      <c r="E2">
+        <v>0.2833173310254271</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <v>2.310833011807985</v>
+      </c>
+      <c r="L2">
+        <v>3.074823677071994</v>
+      </c>
+      <c r="M2">
+        <v>1.87719273784792</v>
+      </c>
+      <c r="N2">
+        <v>2.756514802231027</v>
+      </c>
+      <c r="O2">
+        <v>1.98322131717799</v>
+      </c>
+      <c r="P2">
+        <v>63.87312</v>
+      </c>
+      <c r="Q2">
+        <v>80.6139216240597</v>
+      </c>
+      <c r="R2">
+        <v>48.20646760622282</v>
+      </c>
+      <c r="S2">
+        <v>72.54442600904571</v>
+      </c>
+      <c r="T2">
+        <v>55.01307818624297</v>
+      </c>
+      <c r="U2">
+        <v>0.2036315743238685</v>
+      </c>
+      <c r="V2">
+        <v>0.2682323070472097</v>
+      </c>
+      <c r="W2">
+        <v>0.1496082539444801</v>
+      </c>
+      <c r="X2">
+        <v>0.2357588268069369</v>
+      </c>
+      <c r="Y2">
+        <v>0.1723126592181718</v>
+      </c>
+      <c r="Z2">
+        <v>0.8595681127641212</v>
+      </c>
+      <c r="AA2">
+        <v>0.9214334336684912</v>
+      </c>
+      <c r="AB2">
+        <v>0.7930213729798157</v>
+      </c>
+      <c r="AC2">
+        <v>0.8933934359089717</v>
+      </c>
+      <c r="AD2">
+        <v>0.8229781398733821</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3">
+        <v>0.33</v>
+      </c>
+      <c r="B3">
+        <v>0.33</v>
+      </c>
+      <c r="C3">
+        <v>0.33</v>
+      </c>
+      <c r="D3">
+        <v>0.33</v>
+      </c>
+      <c r="E3">
+        <v>0.33</v>
+      </c>
+      <c r="F3">
+        <v>7.007635130816028</v>
+      </c>
+      <c r="G3">
+        <v>10.66373115801005</v>
+      </c>
+      <c r="H3">
+        <v>4.928011208955038</v>
+      </c>
+      <c r="I3">
+        <v>9.15331336593761</v>
+      </c>
+      <c r="J3">
+        <v>5.432240654920579</v>
+      </c>
+      <c r="K3">
+        <v>2.312519593169289</v>
+      </c>
+      <c r="L3">
+        <v>3.519031282143315</v>
+      </c>
+      <c r="M3">
+        <v>1.626243698955163</v>
+      </c>
+      <c r="N3">
+        <v>3.020593410759412</v>
+      </c>
+      <c r="O3">
+        <v>1.792639416123792</v>
+      </c>
+      <c r="P3">
+        <v>63.86868</v>
+      </c>
+      <c r="Q3">
+        <v>75.29648312914506</v>
+      </c>
+      <c r="R3">
+        <v>55.39346912497681</v>
+      </c>
+      <c r="S3">
+        <v>69.22892118646891</v>
+      </c>
+      <c r="T3">
+        <v>58.90664900779527</v>
+      </c>
+      <c r="U3">
+        <v>0.202351836044429</v>
+      </c>
+      <c r="V3">
+        <v>0.301267351046891</v>
+      </c>
+      <c r="W3">
+        <v>0.1158180784455701</v>
+      </c>
+      <c r="X3">
+        <v>0.2525734092777432</v>
+      </c>
+      <c r="Y3">
+        <v>0.1524643260468851</v>
+      </c>
+      <c r="Z3">
+        <v>0.8527112130544341</v>
+      </c>
+      <c r="AA3">
+        <v>0.9444114918583431</v>
+      </c>
+      <c r="AB3">
+        <v>0.7333842178889807</v>
+      </c>
+      <c r="AC3">
+        <v>0.9053422655933843</v>
+      </c>
+      <c r="AD3">
+        <v>0.7909827579761647</v>
+      </c>
+    </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>0.3300548414179534</v>
+        <v>0.3300101506138201</v>
       </c>
       <c r="B4">
-        <v>0.438391105008159</v>
+        <v>0.4380984843735671</v>
       </c>
       <c r="C4">
-        <v>0.2679979988735469</v>
+        <v>0.2683619067547757</v>
       </c>
       <c r="D4">
-        <v>0.3937391041631541</v>
+        <v>0.3938776276840846</v>
       </c>
       <c r="E4">
-        <v>0.2828853923370157</v>
+        <v>0.2832842281361018</v>
       </c>
       <c r="F4">
-        <v>7.007322609896816</v>
+        <v>7.010519531791773</v>
       </c>
       <c r="G4">
-        <v>10.59244524579269</v>
+        <v>10.58179393613846</v>
       </c>
       <c r="H4">
-        <v>4.943887736082482</v>
+        <v>4.947601034388743</v>
       </c>
       <c r="I4">
-        <v>9.156663608614821</v>
+        <v>9.150958261144595</v>
       </c>
       <c r="J4">
-        <v>5.454697200150446</v>
+        <v>5.447256184493503</v>
       </c>
       <c r="K4">
-        <v>2.312828591780329</v>
+        <v>2.313467379032933</v>
       </c>
       <c r="L4">
-        <v>3.776206511706212</v>
+        <v>3.745063475529567</v>
       </c>
       <c r="M4">
-        <v>1.504166808897832</v>
+        <v>1.506411185974205</v>
       </c>
       <c r="N4">
-        <v>3.157386487208637</v>
+        <v>3.162036401100095</v>
       </c>
       <c r="O4">
-        <v>1.705213153564048</v>
+        <v>1.705080443534392</v>
       </c>
       <c r="P4">
-        <v>65.09828</v>
+        <v>65.09014999999999</v>
       </c>
       <c r="Q4">
-        <v>90.86152396822476</v>
+        <v>90.8111136119704</v>
       </c>
       <c r="R4">
-        <v>47.47755553305626</v>
+        <v>47.4964501604466</v>
       </c>
       <c r="S4">
-        <v>74.3787818779372</v>
+        <v>74.54051024856834</v>
       </c>
       <c r="T4">
-        <v>54.8664087005132</v>
+        <v>54.86208624450914</v>
       </c>
       <c r="U4">
-        <v>0.2014188176078627</v>
+        <v>0.2015309889136741</v>
       </c>
       <c r="V4">
-        <v>0.3170577056105753</v>
+        <v>0.3170041411973542</v>
       </c>
       <c r="W4">
-        <v>0.09951348041250996</v>
+        <v>0.09954999808116222</v>
       </c>
       <c r="X4">
-        <v>0.2601819905801135</v>
+        <v>0.2601609232230361</v>
       </c>
       <c r="Y4">
-        <v>0.1428659134014484</v>
+        <v>0.1430550970729725</v>
       </c>
       <c r="Z4">
-        <v>0.8480062911440618</v>
+        <v>0.8481576253610655</v>
       </c>
       <c r="AA4">
-        <v>0.9544705393367487</v>
+        <v>0.9545503030941668</v>
       </c>
       <c r="AB4">
-        <v>0.6981762718042079</v>
+        <v>0.6980982725575562</v>
       </c>
       <c r="AC4">
-        <v>0.9096999253447704</v>
+        <v>0.9096419629661192</v>
       </c>
       <c r="AD4">
-        <v>0.7729972162013145</v>
+        <v>0.7732800041148812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for streamlines SIR/SEIR monte carlo simulations
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
@@ -19,91 +19,91 @@
     <t>beta-mean</t>
   </si>
   <si>
-    <t>beta-Q99.85</t>
-  </si>
-  <si>
-    <t>beta-Q0.15</t>
+    <t>beta-Q15.5</t>
+  </si>
+  <si>
+    <t>beta-Q83.5</t>
+  </si>
+  <si>
+    <t>beta-Q2.5</t>
   </si>
   <si>
     <t>beta-Q97.5</t>
   </si>
   <si>
-    <t>beta-Q2.5</t>
-  </si>
-  <si>
     <t>gamma-inv-mean</t>
   </si>
   <si>
-    <t>gamma-inv-Q99.85</t>
-  </si>
-  <si>
-    <t>gamma-inv-Q0.15</t>
+    <t>gamma-inv-Q15.5</t>
+  </si>
+  <si>
+    <t>gamma-inv-Q83.5</t>
+  </si>
+  <si>
+    <t>gamma-inv-Q2.5</t>
   </si>
   <si>
     <t>gamma-inv-Q97.5</t>
   </si>
   <si>
-    <t>gamma-inv-Q2.5</t>
-  </si>
-  <si>
     <t>R_0-mean</t>
   </si>
   <si>
-    <t>R_0-Q99.85</t>
-  </si>
-  <si>
-    <t>R_0-Q0.15</t>
+    <t>R_0-Q15.5</t>
+  </si>
+  <si>
+    <t>R_0-Q83.5</t>
+  </si>
+  <si>
+    <t>R_0-Q2.5</t>
   </si>
   <si>
     <t>R_0-Q97.5</t>
   </si>
   <si>
-    <t>R_0-Q2.5</t>
-  </si>
-  <si>
     <t>t_c-mean</t>
   </si>
   <si>
+    <t>t_c-Q15.5</t>
+  </si>
+  <si>
+    <t>t_c-Q83.5</t>
+  </si>
+  <si>
+    <t>t_c-Q2.5</t>
+  </si>
+  <si>
     <t>t_c-Q97.5</t>
   </si>
   <si>
-    <t>t_c-Q2.5</t>
-  </si>
-  <si>
-    <t>t_c-Q83.5</t>
-  </si>
-  <si>
-    <t>t_c-Q15.5</t>
-  </si>
-  <si>
     <t>I_peak-mean</t>
   </si>
   <si>
+    <t>I_peak-Q15.5</t>
+  </si>
+  <si>
+    <t>I_peak-Q83.5</t>
+  </si>
+  <si>
+    <t>I_peak-Q2.5</t>
+  </si>
+  <si>
     <t>I_peak-Q97.5</t>
   </si>
   <si>
-    <t>I_peak-Q2.5</t>
-  </si>
-  <si>
-    <t>I_peak-Q83.5</t>
-  </si>
-  <si>
-    <t>I_peak-Q15.5</t>
-  </si>
-  <si>
     <t>T_end-mean</t>
   </si>
   <si>
+    <t>T_end-Q15.5</t>
+  </si>
+  <si>
+    <t>T_end-Q83.5</t>
+  </si>
+  <si>
+    <t>T_end-Q2.5</t>
+  </si>
+  <si>
     <t>T_end-Q97.5</t>
-  </si>
-  <si>
-    <t>T_end-Q2.5</t>
-  </si>
-  <si>
-    <t>T_end-Q83.5</t>
-  </si>
-  <si>
-    <t>T_end-Q15.5</t>
   </si>
 </sst>
 </file>
@@ -535,19 +535,19 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2">
-        <v>0.330119001686855</v>
+        <v>0.3300499060118708</v>
       </c>
       <c r="B2">
-        <v>0.4392605252959991</v>
+        <v>0.2953613910451203</v>
       </c>
       <c r="C2">
-        <v>0.2681703911211314</v>
+        <v>0.3633580143913455</v>
       </c>
       <c r="D2">
-        <v>0.3937878288901468</v>
+        <v>0.271946956947787</v>
       </c>
       <c r="E2">
-        <v>0.2833173310254271</v>
+        <v>0.4069920332739979</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -565,64 +565,64 @@
         <v>7</v>
       </c>
       <c r="K2">
-        <v>2.310833011807985</v>
+        <v>2.310349342083096</v>
       </c>
       <c r="L2">
-        <v>3.074823677071994</v>
+        <v>2.067529737315842</v>
       </c>
       <c r="M2">
-        <v>1.87719273784792</v>
+        <v>2.543506100739418</v>
       </c>
       <c r="N2">
-        <v>2.756514802231027</v>
+        <v>1.903628698634509</v>
       </c>
       <c r="O2">
-        <v>1.98322131717799</v>
+        <v>2.848944232917985</v>
       </c>
       <c r="P2">
-        <v>63.87312</v>
+        <v>64.48788999999999</v>
       </c>
       <c r="Q2">
-        <v>80.6139216240597</v>
+        <v>46.20353251271484</v>
       </c>
       <c r="R2">
-        <v>48.20646760622282</v>
+        <v>87.6772320006519</v>
       </c>
       <c r="S2">
-        <v>72.54442600904571</v>
+        <v>53.56114539921523</v>
       </c>
       <c r="T2">
-        <v>55.01307818624297</v>
+        <v>74.57462299720029</v>
       </c>
       <c r="U2">
-        <v>0.2036315743238685</v>
+        <v>0.2030477690805852</v>
       </c>
       <c r="V2">
-        <v>0.2682323070472097</v>
+        <v>0.1643481661970219</v>
       </c>
       <c r="W2">
-        <v>0.1496082539444801</v>
+        <v>0.2419927606527416</v>
       </c>
       <c r="X2">
-        <v>0.2357588268069369</v>
+        <v>0.1356656996107907</v>
       </c>
       <c r="Y2">
-        <v>0.1723126592181718</v>
+        <v>0.2800230314464088</v>
       </c>
       <c r="Z2">
-        <v>0.8595681127641212</v>
+        <v>0.8571281783494924</v>
       </c>
       <c r="AA2">
-        <v>0.9214334336684912</v>
+        <v>0.81085013287319</v>
       </c>
       <c r="AB2">
-        <v>0.7930213729798157</v>
+        <v>0.8980873652968309</v>
       </c>
       <c r="AC2">
-        <v>0.8933934359089717</v>
+        <v>0.7700111195685573</v>
       </c>
       <c r="AD2">
-        <v>0.8229781398733821</v>
+        <v>0.9302255099274735</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -642,171 +642,171 @@
         <v>0.33</v>
       </c>
       <c r="F3">
-        <v>7.007635130816028</v>
+        <v>6.997911609327875</v>
       </c>
       <c r="G3">
-        <v>10.66373115801005</v>
+        <v>6.210342225982567</v>
       </c>
       <c r="H3">
-        <v>4.928011208955038</v>
+        <v>7.747438010729122</v>
       </c>
       <c r="I3">
-        <v>9.15331336593761</v>
+        <v>5.693943946463319</v>
       </c>
       <c r="J3">
-        <v>5.432240654920579</v>
+        <v>8.779566248620817</v>
       </c>
       <c r="K3">
-        <v>2.312519593169289</v>
+        <v>2.309310831078199</v>
       </c>
       <c r="L3">
-        <v>3.519031282143315</v>
+        <v>2.049412934574248</v>
       </c>
       <c r="M3">
-        <v>1.626243698955163</v>
+        <v>2.55665454354061</v>
       </c>
       <c r="N3">
-        <v>3.020593410759412</v>
+        <v>1.879001502332895</v>
       </c>
       <c r="O3">
-        <v>1.792639416123792</v>
+        <v>2.89725686204487</v>
       </c>
       <c r="P3">
-        <v>63.86868</v>
+        <v>63.53957</v>
       </c>
       <c r="Q3">
-        <v>75.29648312914506</v>
+        <v>56.39647523232526</v>
       </c>
       <c r="R3">
-        <v>55.39346912497681</v>
+        <v>72.30353979352127</v>
       </c>
       <c r="S3">
-        <v>69.22892118646891</v>
+        <v>59.40480311769122</v>
       </c>
       <c r="T3">
-        <v>58.90664900779527</v>
+        <v>67.82739293048661</v>
       </c>
       <c r="U3">
-        <v>0.202351836044429</v>
+        <v>0.2026521904241902</v>
       </c>
       <c r="V3">
-        <v>0.301267351046891</v>
+        <v>0.1614428624796646</v>
       </c>
       <c r="W3">
-        <v>0.1158180784455701</v>
+        <v>0.2444269455347663</v>
       </c>
       <c r="X3">
-        <v>0.2525734092777432</v>
+        <v>0.1310788822784472</v>
       </c>
       <c r="Y3">
-        <v>0.1524643260468851</v>
+        <v>0.2858611211784558</v>
       </c>
       <c r="Z3">
-        <v>0.8527112130544341</v>
+        <v>0.8558996011535711</v>
       </c>
       <c r="AA3">
-        <v>0.9444114918583431</v>
+        <v>0.8062071331525196</v>
       </c>
       <c r="AB3">
-        <v>0.7333842178889807</v>
+        <v>0.8998128159466621</v>
       </c>
       <c r="AC3">
-        <v>0.9053422655933843</v>
+        <v>0.7623227833969787</v>
       </c>
       <c r="AD3">
-        <v>0.7909827579761647</v>
+        <v>0.9341038326876447</v>
       </c>
     </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>0.3300101506138201</v>
+        <v>0.3300191363416627</v>
       </c>
       <c r="B4">
-        <v>0.4380984843735671</v>
+        <v>0.2953936898295382</v>
       </c>
       <c r="C4">
-        <v>0.2683619067547757</v>
+        <v>0.3631343751871358</v>
       </c>
       <c r="D4">
-        <v>0.3938776276840846</v>
+        <v>0.2719975722997606</v>
       </c>
       <c r="E4">
-        <v>0.2832842281361018</v>
+        <v>0.406778017689316</v>
       </c>
       <c r="F4">
-        <v>7.010519531791773</v>
+        <v>7.00047510005597</v>
       </c>
       <c r="G4">
-        <v>10.58179393613846</v>
+        <v>6.213335460656964</v>
       </c>
       <c r="H4">
-        <v>4.947601034388743</v>
+        <v>7.754827506595099</v>
       </c>
       <c r="I4">
-        <v>9.150958261144595</v>
+        <v>5.69610889909607</v>
       </c>
       <c r="J4">
-        <v>5.447256184493503</v>
+        <v>8.781418602459933</v>
       </c>
       <c r="K4">
-        <v>2.313467379032933</v>
+        <v>2.310420417988074</v>
       </c>
       <c r="L4">
-        <v>3.745063475529567</v>
+        <v>1.957020368334278</v>
       </c>
       <c r="M4">
-        <v>1.506411185974205</v>
+        <v>2.649412775043653</v>
       </c>
       <c r="N4">
-        <v>3.162036401100095</v>
+        <v>1.720654360957462</v>
       </c>
       <c r="O4">
-        <v>1.705080443534392</v>
+        <v>3.113987979913325</v>
       </c>
       <c r="P4">
-        <v>65.09014999999999</v>
+        <v>65.38379999999999</v>
       </c>
       <c r="Q4">
-        <v>90.8111136119704</v>
+        <v>45.5884797976407</v>
       </c>
       <c r="R4">
-        <v>47.4964501604466</v>
+        <v>94.57954781029983</v>
       </c>
       <c r="S4">
-        <v>74.54051024856834</v>
+        <v>53.75743574891678</v>
       </c>
       <c r="T4">
-        <v>54.86208624450914</v>
+        <v>76.64907939477872</v>
       </c>
       <c r="U4">
-        <v>0.2015309889136741</v>
+        <v>0.2013060712975479</v>
       </c>
       <c r="V4">
-        <v>0.3170041411973542</v>
+        <v>0.1448516681886182</v>
       </c>
       <c r="W4">
-        <v>0.09954999808116222</v>
+        <v>0.2578206928040442</v>
       </c>
       <c r="X4">
-        <v>0.2601609232230361</v>
+        <v>0.102701757916482</v>
       </c>
       <c r="Y4">
-        <v>0.1430550970729725</v>
+        <v>0.3125445047127944</v>
       </c>
       <c r="Z4">
-        <v>0.8481576253610655</v>
+        <v>0.8487886733785018</v>
       </c>
       <c r="AA4">
-        <v>0.9545503030941668</v>
+        <v>0.776808401230911</v>
       </c>
       <c r="AB4">
-        <v>0.6980982725575562</v>
+        <v>0.9082350849830558</v>
       </c>
       <c r="AC4">
-        <v>0.9096419629661192</v>
+        <v>0.7052318602969566</v>
       </c>
       <c r="AD4">
-        <v>0.7732800041148812</v>
+        <v>0.9518547260593895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making monte carlo SIR and SEIR tests cohesive
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
@@ -535,19 +535,19 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2">
-        <v>0.3300499060118708</v>
+        <v>0.329814376738541</v>
       </c>
       <c r="B2">
-        <v>0.2953613910451203</v>
+        <v>0.2954230338842676</v>
       </c>
       <c r="C2">
-        <v>0.3633580143913455</v>
+        <v>0.3628265025940295</v>
       </c>
       <c r="D2">
-        <v>0.271946956947787</v>
+        <v>0.2721144324105971</v>
       </c>
       <c r="E2">
-        <v>0.4069920332739979</v>
+        <v>0.4068229258834966</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -565,64 +565,64 @@
         <v>7</v>
       </c>
       <c r="K2">
-        <v>2.310349342083096</v>
+        <v>2.308700637169787</v>
       </c>
       <c r="L2">
-        <v>2.067529737315842</v>
+        <v>2.067961237189873</v>
       </c>
       <c r="M2">
-        <v>2.543506100739418</v>
+        <v>2.539785518158206</v>
       </c>
       <c r="N2">
-        <v>1.903628698634509</v>
+        <v>1.90480102687418</v>
       </c>
       <c r="O2">
-        <v>2.848944232917985</v>
+        <v>2.847760481184476</v>
       </c>
       <c r="P2">
-        <v>64.48788999999999</v>
+        <v>64.54441</v>
       </c>
       <c r="Q2">
-        <v>46.20353251271484</v>
+        <v>46.29748610134416</v>
       </c>
       <c r="R2">
-        <v>87.6772320006519</v>
+        <v>87.42864091694132</v>
       </c>
       <c r="S2">
-        <v>53.56114539921523</v>
+        <v>53.61109968745336</v>
       </c>
       <c r="T2">
-        <v>74.57462299720029</v>
+        <v>74.66188525398353</v>
       </c>
       <c r="U2">
-        <v>0.2030477690805852</v>
+        <v>0.2028046299179496</v>
       </c>
       <c r="V2">
-        <v>0.1643481661970219</v>
+        <v>0.164399412302132</v>
       </c>
       <c r="W2">
-        <v>0.2419927606527416</v>
+        <v>0.2415665995288183</v>
       </c>
       <c r="X2">
-        <v>0.1356656996107907</v>
+        <v>0.1359348926839613</v>
       </c>
       <c r="Y2">
-        <v>0.2800230314464088</v>
+        <v>0.2797384063660836</v>
       </c>
       <c r="Z2">
-        <v>0.8571281783494924</v>
+        <v>0.8569092516457457</v>
       </c>
       <c r="AA2">
-        <v>0.81085013287319</v>
+        <v>0.8109437027015787</v>
       </c>
       <c r="AB2">
-        <v>0.8980873652968309</v>
+        <v>0.8977337412525318</v>
       </c>
       <c r="AC2">
-        <v>0.7700111195685573</v>
+        <v>0.7705067053523447</v>
       </c>
       <c r="AD2">
-        <v>0.9302255099274735</v>
+        <v>0.9300398675239179</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -642,171 +642,171 @@
         <v>0.33</v>
       </c>
       <c r="F3">
-        <v>6.997911609327875</v>
+        <v>7.001189101731514</v>
       </c>
       <c r="G3">
-        <v>6.210342225982567</v>
+        <v>6.212024365265301</v>
       </c>
       <c r="H3">
-        <v>7.747438010729122</v>
+        <v>7.754818811715914</v>
       </c>
       <c r="I3">
-        <v>5.693943946463319</v>
+        <v>5.703289538520241</v>
       </c>
       <c r="J3">
-        <v>8.779566248620817</v>
+        <v>8.785199554711253</v>
       </c>
       <c r="K3">
-        <v>2.309310831078199</v>
+        <v>2.3103924035714</v>
       </c>
       <c r="L3">
-        <v>2.049412934574248</v>
+        <v>2.04996804053755</v>
       </c>
       <c r="M3">
-        <v>2.55665454354061</v>
+        <v>2.559090207866252</v>
       </c>
       <c r="N3">
-        <v>1.879001502332895</v>
+        <v>1.882085547711679</v>
       </c>
       <c r="O3">
-        <v>2.89725686204487</v>
+        <v>2.899115853054714</v>
       </c>
       <c r="P3">
-        <v>63.53957</v>
+        <v>63.52424</v>
       </c>
       <c r="Q3">
-        <v>56.39647523232526</v>
+        <v>56.39283059166551</v>
       </c>
       <c r="R3">
-        <v>72.30353979352127</v>
+        <v>72.2141371691701</v>
       </c>
       <c r="S3">
-        <v>59.40480311769122</v>
+        <v>59.37693894815393</v>
       </c>
       <c r="T3">
-        <v>67.82739293048661</v>
+        <v>67.81250866268077</v>
       </c>
       <c r="U3">
-        <v>0.2026521904241902</v>
+        <v>0.2028134555222862</v>
       </c>
       <c r="V3">
-        <v>0.1614428624796646</v>
+        <v>0.1615561728265415</v>
       </c>
       <c r="W3">
-        <v>0.2444269455347663</v>
+        <v>0.2447438339307111</v>
       </c>
       <c r="X3">
-        <v>0.1310788822784472</v>
+        <v>0.131546783205473</v>
       </c>
       <c r="Y3">
-        <v>0.2858611211784558</v>
+        <v>0.286157498810601</v>
       </c>
       <c r="Z3">
-        <v>0.8558996011535711</v>
+        <v>0.8560805618415306</v>
       </c>
       <c r="AA3">
-        <v>0.8062071331525196</v>
+        <v>0.8064146390035332</v>
       </c>
       <c r="AB3">
-        <v>0.8998128159466621</v>
+        <v>0.9001245295524177</v>
       </c>
       <c r="AC3">
-        <v>0.7623227833969787</v>
+        <v>0.7632224970590397</v>
       </c>
       <c r="AD3">
-        <v>0.9341038326876447</v>
+        <v>0.9341686915997631</v>
       </c>
     </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>0.3300191363416627</v>
+        <v>0.3301008880891508</v>
       </c>
       <c r="B4">
-        <v>0.2953936898295382</v>
+        <v>0.295501325460806</v>
       </c>
       <c r="C4">
-        <v>0.3631343751871358</v>
+        <v>0.3632672235549657</v>
       </c>
       <c r="D4">
-        <v>0.2719975722997606</v>
+        <v>0.2721877960524035</v>
       </c>
       <c r="E4">
-        <v>0.406778017689316</v>
+        <v>0.4070528584374838</v>
       </c>
       <c r="F4">
-        <v>7.00047510005597</v>
+        <v>7.001529098039073</v>
       </c>
       <c r="G4">
-        <v>6.213335460656964</v>
+        <v>6.219226625207799</v>
       </c>
       <c r="H4">
-        <v>7.754827506595099</v>
+        <v>7.753913499864607</v>
       </c>
       <c r="I4">
-        <v>5.69610889909607</v>
+        <v>5.709017536113828</v>
       </c>
       <c r="J4">
-        <v>8.781418602459933</v>
+        <v>8.768311080594755</v>
       </c>
       <c r="K4">
-        <v>2.310420417988074</v>
+        <v>2.311371204970385</v>
       </c>
       <c r="L4">
-        <v>1.957020368334278</v>
+        <v>1.959791563416804</v>
       </c>
       <c r="M4">
-        <v>2.649412775043653</v>
+        <v>2.650350248252937</v>
       </c>
       <c r="N4">
-        <v>1.720654360957462</v>
+        <v>1.721624650984149</v>
       </c>
       <c r="O4">
-        <v>3.113987979913325</v>
+        <v>3.117795841065266</v>
       </c>
       <c r="P4">
-        <v>65.38379999999999</v>
+        <v>65.34237</v>
       </c>
       <c r="Q4">
-        <v>45.5884797976407</v>
+        <v>45.59072657740801</v>
       </c>
       <c r="R4">
-        <v>94.57954781029983</v>
+        <v>94.65279409933459</v>
       </c>
       <c r="S4">
-        <v>53.75743574891678</v>
+        <v>53.69611793254276</v>
       </c>
       <c r="T4">
-        <v>76.64907939477872</v>
+        <v>76.44578313582664</v>
       </c>
       <c r="U4">
-        <v>0.2013060712975479</v>
+        <v>0.2014640536348754</v>
       </c>
       <c r="V4">
-        <v>0.1448516681886182</v>
+        <v>0.1451732985503876</v>
       </c>
       <c r="W4">
-        <v>0.2578206928040442</v>
+        <v>0.2578642589046234</v>
       </c>
       <c r="X4">
-        <v>0.102701757916482</v>
+        <v>0.1030804296677801</v>
       </c>
       <c r="Y4">
-        <v>0.3125445047127944</v>
+        <v>0.3126961887145306</v>
       </c>
       <c r="Z4">
-        <v>0.8487886733785018</v>
+        <v>0.8490192072278532</v>
       </c>
       <c r="AA4">
-        <v>0.776808401230911</v>
+        <v>0.7773669948036431</v>
       </c>
       <c r="AB4">
-        <v>0.9082350849830558</v>
+        <v>0.908221349716789</v>
       </c>
       <c r="AC4">
-        <v>0.7052318602969566</v>
+        <v>0.7058395560397965</v>
       </c>
       <c r="AD4">
-        <v>0.9518547260593895</v>
+        <v>0.9520788124809904</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monte carlo tests updates section 4
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_gamma.xlsx
@@ -535,19 +535,19 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2">
-        <v>0.329814376738541</v>
+        <v>0.3301315503884687</v>
       </c>
       <c r="B2">
-        <v>0.2954230338842676</v>
+        <v>0.2955902794325816</v>
       </c>
       <c r="C2">
-        <v>0.3628265025940295</v>
+        <v>0.3630767971809157</v>
       </c>
       <c r="D2">
-        <v>0.2721144324105971</v>
+        <v>0.2725162596895327</v>
       </c>
       <c r="E2">
-        <v>0.4068229258834966</v>
+        <v>0.4066187414426702</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -565,64 +565,64 @@
         <v>7</v>
       </c>
       <c r="K2">
-        <v>2.308700637169787</v>
+        <v>2.31092085271928</v>
       </c>
       <c r="L2">
-        <v>2.067961237189873</v>
+        <v>2.069131956028071</v>
       </c>
       <c r="M2">
-        <v>2.539785518158206</v>
+        <v>2.54153758026641</v>
       </c>
       <c r="N2">
-        <v>1.90480102687418</v>
+        <v>1.907613817826729</v>
       </c>
       <c r="O2">
-        <v>2.847760481184476</v>
+        <v>2.846331190098691</v>
       </c>
       <c r="P2">
-        <v>64.54441</v>
+        <v>64.44223</v>
       </c>
       <c r="Q2">
-        <v>46.29748610134416</v>
+        <v>46.30304518419486</v>
       </c>
       <c r="R2">
-        <v>87.42864091694132</v>
+        <v>87.33486795507919</v>
       </c>
       <c r="S2">
-        <v>53.61109968745336</v>
+        <v>53.5777423435626</v>
       </c>
       <c r="T2">
-        <v>74.66188525398353</v>
+        <v>74.5312578753298</v>
       </c>
       <c r="U2">
-        <v>0.2028046299179496</v>
+        <v>0.2031548274478529</v>
       </c>
       <c r="V2">
-        <v>0.164399412302132</v>
+        <v>0.164662504147416</v>
       </c>
       <c r="W2">
-        <v>0.2415665995288183</v>
+        <v>0.241878409505886</v>
       </c>
       <c r="X2">
-        <v>0.1359348926839613</v>
+        <v>0.1361939362162032</v>
       </c>
       <c r="Y2">
-        <v>0.2797384063660836</v>
+        <v>0.2795835804766086</v>
       </c>
       <c r="Z2">
-        <v>0.8569092516457457</v>
+        <v>0.8573167908766585</v>
       </c>
       <c r="AA2">
-        <v>0.8109437027015787</v>
+        <v>0.8113466238081585</v>
       </c>
       <c r="AB2">
-        <v>0.8977337412525318</v>
+        <v>0.8980344071975621</v>
       </c>
       <c r="AC2">
-        <v>0.7705067053523447</v>
+        <v>0.7709565353244547</v>
       </c>
       <c r="AD2">
-        <v>0.9300398675239179</v>
+        <v>0.9298609587351283</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -642,171 +642,171 @@
         <v>0.33</v>
       </c>
       <c r="F3">
-        <v>7.001189101731514</v>
+        <v>7.001534600731914</v>
       </c>
       <c r="G3">
-        <v>6.212024365265301</v>
+        <v>6.220797888576329</v>
       </c>
       <c r="H3">
-        <v>7.754818811715914</v>
+        <v>7.754317288312638</v>
       </c>
       <c r="I3">
-        <v>5.703289538520241</v>
+        <v>5.698442768810907</v>
       </c>
       <c r="J3">
-        <v>8.785199554711253</v>
+        <v>8.7717687647198</v>
       </c>
       <c r="K3">
-        <v>2.3103924035714</v>
+        <v>2.310506418241533</v>
       </c>
       <c r="L3">
-        <v>2.04996804053755</v>
+        <v>2.052863303230189</v>
       </c>
       <c r="M3">
-        <v>2.559090207866252</v>
+        <v>2.558924705143171</v>
       </c>
       <c r="N3">
-        <v>1.882085547711679</v>
+        <v>1.880486113707599</v>
       </c>
       <c r="O3">
-        <v>2.899115853054714</v>
+        <v>2.894683692357535</v>
       </c>
       <c r="P3">
-        <v>63.52424</v>
+        <v>63.51508</v>
       </c>
       <c r="Q3">
-        <v>56.39283059166551</v>
+        <v>56.40103009049271</v>
       </c>
       <c r="R3">
-        <v>72.2141371691701</v>
+        <v>72.22926416319957</v>
       </c>
       <c r="S3">
-        <v>59.37693894815393</v>
+        <v>59.40179431101897</v>
       </c>
       <c r="T3">
-        <v>67.81250866268077</v>
+        <v>67.77768657085397</v>
       </c>
       <c r="U3">
-        <v>0.2028134555222862</v>
+        <v>0.2028513684196727</v>
       </c>
       <c r="V3">
-        <v>0.1615561728265415</v>
+        <v>0.1617836624909226</v>
       </c>
       <c r="W3">
-        <v>0.2447438339307111</v>
+        <v>0.2444918034730678</v>
       </c>
       <c r="X3">
-        <v>0.131546783205473</v>
+        <v>0.131574774878728</v>
       </c>
       <c r="Y3">
-        <v>0.286157498810601</v>
+        <v>0.2857563357823072</v>
       </c>
       <c r="Z3">
-        <v>0.8560805618415306</v>
+        <v>0.856172181610088</v>
       </c>
       <c r="AA3">
-        <v>0.8064146390035332</v>
+        <v>0.8067508856446146</v>
       </c>
       <c r="AB3">
-        <v>0.9001245295524177</v>
+        <v>0.8998751425036341</v>
       </c>
       <c r="AC3">
-        <v>0.7632224970590397</v>
+        <v>0.7631267830679144</v>
       </c>
       <c r="AD3">
-        <v>0.9341686915997631</v>
+        <v>0.9340652383046261</v>
       </c>
     </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>0.3301008880891508</v>
+        <v>0.3299527873842167</v>
       </c>
       <c r="B4">
-        <v>0.295501325460806</v>
+        <v>0.2955532292028652</v>
       </c>
       <c r="C4">
-        <v>0.3632672235549657</v>
+        <v>0.3629908133231589</v>
       </c>
       <c r="D4">
-        <v>0.2721877960524035</v>
+        <v>0.2719585148209576</v>
       </c>
       <c r="E4">
-        <v>0.4070528584374838</v>
+        <v>0.4067924091754813</v>
       </c>
       <c r="F4">
-        <v>7.001529098039073</v>
+        <v>7.003102622518629</v>
       </c>
       <c r="G4">
-        <v>6.219226625207799</v>
+        <v>6.217063611490602</v>
       </c>
       <c r="H4">
-        <v>7.753913499864607</v>
+        <v>7.758896798529163</v>
       </c>
       <c r="I4">
-        <v>5.709017536113828</v>
+        <v>5.700984323911813</v>
       </c>
       <c r="J4">
-        <v>8.768311080594755</v>
+        <v>8.774824090174556</v>
       </c>
       <c r="K4">
-        <v>2.311371204970385</v>
+        <v>2.310581376869882</v>
       </c>
       <c r="L4">
-        <v>1.959791563416804</v>
+        <v>1.960099274045088</v>
       </c>
       <c r="M4">
-        <v>2.650350248252937</v>
+        <v>2.647115016992029</v>
       </c>
       <c r="N4">
-        <v>1.721624650984149</v>
+        <v>1.725673933688124</v>
       </c>
       <c r="O4">
-        <v>3.117795841065266</v>
+        <v>3.109328671323687</v>
       </c>
       <c r="P4">
-        <v>65.34237</v>
+        <v>65.36592</v>
       </c>
       <c r="Q4">
-        <v>45.59072657740801</v>
+        <v>45.65299091608324</v>
       </c>
       <c r="R4">
-        <v>94.65279409933459</v>
+        <v>94.4306790924532</v>
       </c>
       <c r="S4">
-        <v>53.69611793254276</v>
+        <v>53.76457611257006</v>
       </c>
       <c r="T4">
-        <v>76.44578313582664</v>
+        <v>76.43869195732356</v>
       </c>
       <c r="U4">
-        <v>0.2014640536348754</v>
+        <v>0.2013647291966062</v>
       </c>
       <c r="V4">
-        <v>0.1451732985503876</v>
+        <v>0.14530336231264</v>
       </c>
       <c r="W4">
-        <v>0.2578642589046234</v>
+        <v>0.2575543796331879</v>
       </c>
       <c r="X4">
-        <v>0.1030804296677801</v>
+        <v>0.1034315077128284</v>
       </c>
       <c r="Y4">
-        <v>0.3126961887145306</v>
+        <v>0.3121750978671887</v>
       </c>
       <c r="Z4">
-        <v>0.8490192072278532</v>
+        <v>0.8490013627832288</v>
       </c>
       <c r="AA4">
-        <v>0.7773669948036431</v>
+        <v>0.7776481050978237</v>
       </c>
       <c r="AB4">
-        <v>0.908221349716789</v>
+        <v>0.9080409396528987</v>
       </c>
       <c r="AC4">
-        <v>0.7058395560397965</v>
+        <v>0.7066943562492456</v>
       </c>
       <c r="AD4">
-        <v>0.9520788124809904</v>
+        <v>0.9517019068147211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>